<commit_message>
added more physics to tutorial scene
</commit_message>
<xml_diff>
--- a/ToDo/ToDoList.xlsx
+++ b/ToDo/ToDoList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annag\Documents\GitHub\CS-4455-Spr-2018-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annag\Documents\GitHub\CS-4455-Spr-2018-Project\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8058DDE1-F640-4D91-B00F-7E501F3FEA03}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B586921-3302-4FDF-A3C2-4E5E79E9A8D7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{97D0CD48-1E1F-46CF-A005-D26AF7ED2C5C}"/>
   </bookViews>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -161,11 +161,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A269BAD-0741-421F-B3F2-F126B94B48BC}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -510,7 +511,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -522,12 +523,12 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">

</xml_diff>